<commit_message>
Developed a test and added line spaces
</commit_message>
<xml_diff>
--- a/coxaxle/src/test/resources/datasheets/AT_08_VerifyUpdateContacts.xlsx
+++ b/coxaxle/src/test/resources/datasheets/AT_08_VerifyUpdateContacts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Email</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>1234567890</t>
+  </si>
+  <si>
+    <t>ImagePath</t>
+  </si>
+  <si>
+    <t>C:/Users/Public/Pictures/Sample Pictures/Penguins.jpg</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -448,9 +454,10 @@
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +485,11 @@
       <c r="I1" t="s">
         <v>12</v>
       </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -506,6 +516,9 @@
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developed test AT_11,Added new page classes
</commit_message>
<xml_diff>
--- a/coxaxle/src/test/resources/datasheets/AT_08_VerifyUpdateContacts.xlsx
+++ b/coxaxle/src/test/resources/datasheets/AT_08_VerifyUpdateContacts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Email</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>C:/Users/Public/Pictures/Sample Pictures/Penguins.jpg</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+  </si>
+  <si>
+    <t>QA789</t>
   </si>
 </sst>
 </file>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -455,9 +461,10 @@
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +495,11 @@
       <c r="J1" t="s">
         <v>14</v>
       </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -519,6 +529,9 @@
       </c>
       <c r="J2" t="s">
         <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>